<commit_message>
Added exp order files w mono cues
</commit_message>
<xml_diff>
--- a/Experiment/Orders_PILOT/PAR01_RUN02.xlsx
+++ b/Experiment/Orders_PILOT/PAR01_RUN02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24424"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VisionLab\Desktop\3DFaces\Scan Orders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VisionLab\OneDrive - The University of Western Ontario\3DFaces_MD_2020\Scanning\Task\Scan Orders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{4789688D-DCB9-428C-A48A-B845A867EC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{477B918C-17C8-4E84-A896-ADE3BDE5768A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22130E2D-4CFF-4AE4-9954-FF5B6977BC21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4890" windowWidth="29040" windowHeight="15840" xr2:uid="{A9454398-0550-47ED-830A-00A242C6E983}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A9454398-0550-47ED-830A-00A242C6E983}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="60">
   <si>
     <t>Trial</t>
   </si>
@@ -205,13 +205,22 @@
   </si>
   <si>
     <t>Pseudo</t>
+  </si>
+  <si>
+    <t>CUE</t>
+  </si>
+  <si>
+    <t>CoverCue.jpg</t>
+  </si>
+  <si>
+    <t>UncoverCue.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -570,24 +579,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C61BF3D-73CE-4BC2-BEFE-48BC31D9D1BC}">
-  <dimension ref="A1:F202"/>
+  <dimension ref="A1:F206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G216" sqref="G216"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="16" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -618,7 +627,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -638,7 +647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -658,7 +667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -678,7 +687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -698,7 +707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -718,7 +727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -738,7 +747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -758,7 +767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -778,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -798,7 +807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -818,7 +827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -838,7 +847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -858,7 +867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -878,7 +887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -898,7 +907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -918,7 +927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -938,7 +947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -958,7 +967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -978,7 +987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -998,7 +1007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1018,7 +1027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1038,7 +1047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1058,7 +1067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1078,7 +1087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1098,36 +1107,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="3">
+        <v>5</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C28" s="3">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28">
-        <v>2</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="3">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1138,14 +1151,14 @@
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1156,14 +1169,14 @@
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1174,14 +1187,14 @@
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2</v>
       </c>
@@ -1192,14 +1205,14 @@
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2</v>
       </c>
@@ -1210,14 +1223,14 @@
         <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2</v>
       </c>
@@ -1228,14 +1241,14 @@
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2</v>
       </c>
@@ -1246,14 +1259,14 @@
         <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2</v>
       </c>
@@ -1264,14 +1277,14 @@
         <v>1</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1282,14 +1295,14 @@
         <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2</v>
       </c>
@@ -1300,14 +1313,14 @@
         <v>1</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1318,14 +1331,14 @@
         <v>1</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2</v>
       </c>
@@ -1336,14 +1349,14 @@
         <v>1</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2</v>
       </c>
@@ -1354,14 +1367,14 @@
         <v>1</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2</v>
       </c>
@@ -1372,14 +1385,14 @@
         <v>1</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2</v>
       </c>
@@ -1390,14 +1403,14 @@
         <v>1</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2</v>
       </c>
@@ -1408,14 +1421,14 @@
         <v>1</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1433,7 +1446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2</v>
       </c>
@@ -1444,14 +1457,14 @@
         <v>1</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2</v>
       </c>
@@ -1462,14 +1475,14 @@
         <v>1</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2</v>
       </c>
@@ -1480,14 +1493,14 @@
         <v>1</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2</v>
       </c>
@@ -1498,14 +1511,14 @@
         <v>1</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2</v>
       </c>
@@ -1516,14 +1529,14 @@
         <v>1</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2</v>
       </c>
@@ -1534,65 +1547,63 @@
         <v>1</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>0</v>
-      </c>
-      <c r="B52" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="3">
+        <v>1</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" s="1"/>
+      <c r="F52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>0</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" s="3">
+        <v>5</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>0</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C54" s="3">
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
-      <c r="A53">
-        <v>3</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C53" s="3">
-        <v>1</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F53" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54">
-        <v>3</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C54" s="3">
-        <v>1</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F54" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>3</v>
       </c>
@@ -1603,16 +1614,16 @@
         <v>1</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="F55" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>3</v>
       </c>
@@ -1623,16 +1634,16 @@
         <v>1</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F56" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>3</v>
       </c>
@@ -1643,16 +1654,16 @@
         <v>1</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="F57" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>3</v>
       </c>
@@ -1663,16 +1674,16 @@
         <v>1</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F58" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>3</v>
       </c>
@@ -1683,16 +1694,16 @@
         <v>1</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F59" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>3</v>
       </c>
@@ -1703,16 +1714,16 @@
         <v>1</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F60" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>3</v>
       </c>
@@ -1723,16 +1734,16 @@
         <v>1</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F61" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>3</v>
       </c>
@@ -1743,16 +1754,16 @@
         <v>1</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="F62" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>3</v>
       </c>
@@ -1763,16 +1774,16 @@
         <v>1</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="F63" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>3</v>
       </c>
@@ -1783,16 +1794,16 @@
         <v>1</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F64" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>3</v>
       </c>
@@ -1803,16 +1814,16 @@
         <v>1</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="F65" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>3</v>
       </c>
@@ -1823,16 +1834,16 @@
         <v>1</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F66" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>3</v>
       </c>
@@ -1843,16 +1854,16 @@
         <v>1</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F67" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>3</v>
       </c>
@@ -1863,16 +1874,16 @@
         <v>1</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="F68" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>3</v>
       </c>
@@ -1883,16 +1894,16 @@
         <v>1</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="F69" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>3</v>
       </c>
@@ -1903,16 +1914,16 @@
         <v>1</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="F70" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>3</v>
       </c>
@@ -1923,16 +1934,16 @@
         <v>1</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F71" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>3</v>
       </c>
@@ -1943,16 +1954,16 @@
         <v>1</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F72" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>3</v>
       </c>
@@ -1963,16 +1974,16 @@
         <v>1</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F73" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>3</v>
       </c>
@@ -1983,16 +1994,16 @@
         <v>1</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="F74" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>3</v>
       </c>
@@ -2003,16 +2014,16 @@
         <v>1</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="F75" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>3</v>
       </c>
@@ -2023,67 +2034,67 @@
         <v>1</v>
       </c>
       <c r="D76" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>3</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C77" s="3">
+        <v>1</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>3</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C78" s="3">
+        <v>1</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="E78" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F76" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77">
-        <v>0</v>
-      </c>
-      <c r="B77" s="1" t="s">
+      <c r="F78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>0</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C77" s="3">
+      <c r="C79" s="3">
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
-      <c r="A78">
-        <v>4</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C78" s="3">
-        <v>1</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F78" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79">
-        <v>4</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C79" s="3">
-        <v>1</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F79" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>4</v>
       </c>
@@ -2094,16 +2105,16 @@
         <v>1</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F80" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>4</v>
       </c>
@@ -2114,16 +2125,16 @@
         <v>1</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F81" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>4</v>
       </c>
@@ -2134,16 +2145,16 @@
         <v>1</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F82" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>4</v>
       </c>
@@ -2154,16 +2165,16 @@
         <v>1</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="F83" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>4</v>
       </c>
@@ -2174,16 +2185,16 @@
         <v>1</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="F84" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>4</v>
       </c>
@@ -2194,16 +2205,16 @@
         <v>1</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F85" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>4</v>
       </c>
@@ -2214,16 +2225,16 @@
         <v>1</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F86" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>4</v>
       </c>
@@ -2234,16 +2245,16 @@
         <v>1</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="F87" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>4</v>
       </c>
@@ -2254,16 +2265,16 @@
         <v>1</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F88" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>4</v>
       </c>
@@ -2274,16 +2285,16 @@
         <v>1</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="F89" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>4</v>
       </c>
@@ -2294,16 +2305,16 @@
         <v>1</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="F90" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>4</v>
       </c>
@@ -2314,16 +2325,16 @@
         <v>1</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F91" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>4</v>
       </c>
@@ -2334,16 +2345,16 @@
         <v>1</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F92" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>4</v>
       </c>
@@ -2354,16 +2365,16 @@
         <v>1</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="F93" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>4</v>
       </c>
@@ -2374,16 +2385,16 @@
         <v>1</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="F94" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>4</v>
       </c>
@@ -2394,16 +2405,16 @@
         <v>1</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="F95" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>4</v>
       </c>
@@ -2414,16 +2425,16 @@
         <v>1</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="F96" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>4</v>
       </c>
@@ -2434,16 +2445,16 @@
         <v>1</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="F97" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>4</v>
       </c>
@@ -2454,16 +2465,16 @@
         <v>1</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="F98" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>4</v>
       </c>
@@ -2474,16 +2485,16 @@
         <v>1</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F99" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>4</v>
       </c>
@@ -2494,16 +2505,16 @@
         <v>1</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F100" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>4</v>
       </c>
@@ -2514,81 +2525,89 @@
         <v>1</v>
       </c>
       <c r="D101" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>4</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C102" s="3">
+        <v>1</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>4</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C103" s="3">
+        <v>1</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E101" s="1" t="s">
+      <c r="E103" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F101" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6">
-      <c r="A102">
-        <v>0</v>
-      </c>
-      <c r="B102" s="1" t="s">
+      <c r="F103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>0</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C104" s="3">
+        <v>5</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>0</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="3">
+      <c r="C105" s="3">
         <v>24</v>
       </c>
-    </row>
-    <row r="103" spans="1:6">
-      <c r="A103">
-        <v>5</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C103" s="3">
-        <v>1</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E103" s="1"/>
-      <c r="F103" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6">
-      <c r="A104">
-        <v>5</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C104" s="3">
-        <v>1</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E104" s="1"/>
-      <c r="F104" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6">
-      <c r="A105">
-        <v>5</v>
-      </c>
-      <c r="B105" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C105" s="3">
-        <v>1</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="D105" s="1"/>
       <c r="E105" s="1"/>
-      <c r="F105" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6">
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>5</v>
       </c>
@@ -2599,14 +2618,14 @@
         <v>1</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>5</v>
       </c>
@@ -2617,14 +2636,14 @@
         <v>1</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>5</v>
       </c>
@@ -2635,14 +2654,14 @@
         <v>1</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E108" s="1"/>
       <c r="F108" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>5</v>
       </c>
@@ -2653,14 +2672,14 @@
         <v>1</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>5</v>
       </c>
@@ -2671,14 +2690,14 @@
         <v>1</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="E110" s="1"/>
       <c r="F110" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>5</v>
       </c>
@@ -2689,14 +2708,14 @@
         <v>1</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E111" s="1"/>
       <c r="F111" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>5</v>
       </c>
@@ -2707,14 +2726,14 @@
         <v>1</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E112" s="1"/>
       <c r="F112" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>5</v>
       </c>
@@ -2725,14 +2744,14 @@
         <v>1</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E113" s="1"/>
       <c r="F113" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>5</v>
       </c>
@@ -2743,14 +2762,14 @@
         <v>1</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E114" s="1"/>
       <c r="F114" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>5</v>
       </c>
@@ -2761,14 +2780,14 @@
         <v>1</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>5</v>
       </c>
@@ -2779,14 +2798,14 @@
         <v>1</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>5</v>
       </c>
@@ -2797,14 +2816,14 @@
         <v>1</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>5</v>
       </c>
@@ -2815,14 +2834,14 @@
         <v>1</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>5</v>
       </c>
@@ -2833,14 +2852,14 @@
         <v>1</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E119" s="1"/>
       <c r="F119" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>5</v>
       </c>
@@ -2851,14 +2870,14 @@
         <v>1</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="E120" s="1"/>
       <c r="F120" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>5</v>
       </c>
@@ -2869,14 +2888,14 @@
         <v>1</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E121" s="1"/>
       <c r="F121" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>5</v>
       </c>
@@ -2887,14 +2906,14 @@
         <v>1</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="E122" s="1"/>
       <c r="F122" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>5</v>
       </c>
@@ -2905,14 +2924,14 @@
         <v>1</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="E123" s="1"/>
       <c r="F123" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>5</v>
       </c>
@@ -2923,14 +2942,14 @@
         <v>1</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="E124" s="1"/>
       <c r="F124" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>5</v>
       </c>
@@ -2941,14 +2960,14 @@
         <v>1</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>5</v>
       </c>
@@ -2959,105 +2978,101 @@
         <v>1</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>0</v>
-      </c>
-      <c r="B127" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C127" s="3">
+        <v>1</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E127" s="1"/>
+      <c r="F127" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>5</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C128" s="3">
+        <v>1</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E128" s="1"/>
+      <c r="F128" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>5</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C129" s="3">
+        <v>1</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E129" s="1"/>
+      <c r="F129" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>0</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C130" s="3">
+        <v>5</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F130" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>0</v>
+      </c>
+      <c r="B131" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C127" s="3">
+      <c r="C131" s="3">
         <v>24</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" ht="15">
-      <c r="A128">
-        <v>6</v>
-      </c>
-      <c r="B128" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C128" s="3">
-        <v>1</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F128" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6">
-      <c r="A129">
-        <v>6</v>
-      </c>
-      <c r="B129" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C129" s="3">
-        <v>1</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F129" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6">
-      <c r="A130">
-        <v>6</v>
-      </c>
-      <c r="B130" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C130" s="3">
-        <v>1</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E130" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F130" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6">
-      <c r="A131">
-        <v>6</v>
-      </c>
-      <c r="B131" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C131" s="3">
-        <v>1</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F131" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6">
+      <c r="D131" s="1"/>
+      <c r="E131" s="1"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>6</v>
       </c>
@@ -3068,16 +3083,16 @@
         <v>1</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F132" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>6</v>
       </c>
@@ -3088,16 +3103,16 @@
         <v>1</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="F133" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>6</v>
       </c>
@@ -3108,16 +3123,16 @@
         <v>1</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F134" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>6</v>
       </c>
@@ -3128,16 +3143,16 @@
         <v>1</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F135" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>6</v>
       </c>
@@ -3148,16 +3163,16 @@
         <v>1</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F136" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>6</v>
       </c>
@@ -3168,16 +3183,16 @@
         <v>1</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F137" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>6</v>
       </c>
@@ -3188,16 +3203,16 @@
         <v>1</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="F138" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>6</v>
       </c>
@@ -3208,16 +3223,16 @@
         <v>1</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="F139" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>6</v>
       </c>
@@ -3228,16 +3243,16 @@
         <v>1</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="F140" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>6</v>
       </c>
@@ -3248,16 +3263,16 @@
         <v>1</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="F141" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>6</v>
       </c>
@@ -3268,16 +3283,16 @@
         <v>1</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F142" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>6</v>
       </c>
@@ -3288,16 +3303,16 @@
         <v>1</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F143" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>6</v>
       </c>
@@ -3308,16 +3323,16 @@
         <v>1</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="F144" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>6</v>
       </c>
@@ -3328,16 +3343,16 @@
         <v>1</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F145" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>6</v>
       </c>
@@ -3348,16 +3363,16 @@
         <v>1</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F146" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>6</v>
       </c>
@@ -3368,16 +3383,16 @@
         <v>1</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F147" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>6</v>
       </c>
@@ -3388,16 +3403,16 @@
         <v>1</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F148" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>6</v>
       </c>
@@ -3408,16 +3423,16 @@
         <v>1</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F149" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>6</v>
       </c>
@@ -3428,16 +3443,16 @@
         <v>1</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="F150" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>6</v>
       </c>
@@ -3448,563 +3463,572 @@
         <v>1</v>
       </c>
       <c r="D151" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F151" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>6</v>
+      </c>
+      <c r="B152" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C152" s="3">
+        <v>1</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F152" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>6</v>
+      </c>
+      <c r="B153" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C153" s="3">
+        <v>1</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F153" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>6</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C154" s="3">
+        <v>1</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F154" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>6</v>
+      </c>
+      <c r="B155" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C155" s="3">
+        <v>1</v>
+      </c>
+      <c r="D155" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E151" s="1" t="s">
+      <c r="E155" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F151" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6">
-      <c r="A152">
-        <v>0</v>
-      </c>
-      <c r="B152" s="1" t="s">
+      <c r="F155" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>0</v>
+      </c>
+      <c r="B156" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C152" s="3">
+      <c r="C156" s="3">
         <v>24</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
-      <c r="A153">
-        <v>7</v>
-      </c>
-      <c r="B153" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C153" s="3">
-        <v>1</v>
-      </c>
-      <c r="D153" s="1" t="s">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>7</v>
+      </c>
+      <c r="B157" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C157" s="3">
+        <v>1</v>
+      </c>
+      <c r="D157" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E153" s="1" t="s">
+      <c r="E157" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F153" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6">
-      <c r="A154">
-        <v>7</v>
-      </c>
-      <c r="B154" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C154" s="3">
-        <v>1</v>
-      </c>
-      <c r="D154" s="1" t="s">
+      <c r="F157" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>7</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C158" s="3">
+        <v>1</v>
+      </c>
+      <c r="D158" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E154" s="1" t="s">
+      <c r="E158" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F154" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6">
-      <c r="A155">
-        <v>7</v>
-      </c>
-      <c r="B155" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C155" s="3">
-        <v>1</v>
-      </c>
-      <c r="D155" s="1" t="s">
+      <c r="F158" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>7</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C159" s="3">
+        <v>1</v>
+      </c>
+      <c r="D159" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E155" s="1" t="s">
+      <c r="E159" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F155" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6">
-      <c r="A156">
-        <v>7</v>
-      </c>
-      <c r="B156" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C156" s="3">
-        <v>1</v>
-      </c>
-      <c r="D156" s="1" t="s">
+      <c r="F159" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>7</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C160" s="3">
+        <v>1</v>
+      </c>
+      <c r="D160" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E156" s="1" t="s">
+      <c r="E160" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F156" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6">
-      <c r="A157">
-        <v>7</v>
-      </c>
-      <c r="B157" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C157" s="3">
-        <v>1</v>
-      </c>
-      <c r="D157" s="1" t="s">
+      <c r="F160" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>7</v>
+      </c>
+      <c r="B161" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C161" s="3">
+        <v>1</v>
+      </c>
+      <c r="D161" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E157" s="1" t="s">
+      <c r="E161" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F157" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6">
-      <c r="A158">
-        <v>7</v>
-      </c>
-      <c r="B158" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C158" s="3">
-        <v>1</v>
-      </c>
-      <c r="D158" s="1" t="s">
+      <c r="F161" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>7</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C162" s="3">
+        <v>1</v>
+      </c>
+      <c r="D162" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E158" s="1" t="s">
+      <c r="E162" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F158" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6">
-      <c r="A159">
-        <v>7</v>
-      </c>
-      <c r="B159" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C159" s="3">
-        <v>1</v>
-      </c>
-      <c r="D159" s="1" t="s">
+      <c r="F162" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>7</v>
+      </c>
+      <c r="B163" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C163" s="3">
+        <v>1</v>
+      </c>
+      <c r="D163" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E159" s="1" t="s">
+      <c r="E163" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F159" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6">
-      <c r="A160">
-        <v>7</v>
-      </c>
-      <c r="B160" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C160" s="3">
-        <v>1</v>
-      </c>
-      <c r="D160" s="1" t="s">
+      <c r="F163" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <v>7</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C164" s="3">
+        <v>1</v>
+      </c>
+      <c r="D164" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E160" s="1" t="s">
+      <c r="E164" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F160" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6">
-      <c r="A161">
-        <v>7</v>
-      </c>
-      <c r="B161" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C161" s="3">
-        <v>1</v>
-      </c>
-      <c r="D161" s="1" t="s">
+      <c r="F164" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <v>7</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C165" s="3">
+        <v>1</v>
+      </c>
+      <c r="D165" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E161" s="1" t="s">
+      <c r="E165" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F161" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6">
-      <c r="A162">
-        <v>7</v>
-      </c>
-      <c r="B162" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C162" s="3">
-        <v>1</v>
-      </c>
-      <c r="D162" s="1" t="s">
+      <c r="F165" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>7</v>
+      </c>
+      <c r="B166" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C166" s="3">
+        <v>1</v>
+      </c>
+      <c r="D166" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E162" s="1" t="s">
+      <c r="E166" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F162" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6">
-      <c r="A163">
-        <v>7</v>
-      </c>
-      <c r="B163" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C163" s="3">
-        <v>1</v>
-      </c>
-      <c r="D163" s="1" t="s">
+      <c r="F166" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <v>7</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C167" s="3">
+        <v>1</v>
+      </c>
+      <c r="D167" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E163" s="1" t="s">
+      <c r="E167" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F163" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6">
-      <c r="A164">
-        <v>7</v>
-      </c>
-      <c r="B164" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C164" s="3">
-        <v>1</v>
-      </c>
-      <c r="D164" s="1" t="s">
+      <c r="F167" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <v>7</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C168" s="3">
+        <v>1</v>
+      </c>
+      <c r="D168" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E164" s="1" t="s">
+      <c r="E168" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F164" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6">
-      <c r="A165">
-        <v>7</v>
-      </c>
-      <c r="B165" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C165" s="3">
-        <v>1</v>
-      </c>
-      <c r="D165" s="1" t="s">
+      <c r="F168" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>7</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C169" s="3">
+        <v>1</v>
+      </c>
+      <c r="D169" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E165" s="1" t="s">
+      <c r="E169" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F165" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6">
-      <c r="A166">
-        <v>7</v>
-      </c>
-      <c r="B166" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C166" s="3">
-        <v>1</v>
-      </c>
-      <c r="D166" s="1" t="s">
+      <c r="F169" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>7</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C170" s="3">
+        <v>1</v>
+      </c>
+      <c r="D170" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E166" s="1" t="s">
+      <c r="E170" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F166" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6">
-      <c r="A167">
-        <v>7</v>
-      </c>
-      <c r="B167" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C167" s="3">
-        <v>1</v>
-      </c>
-      <c r="D167" s="1" t="s">
+      <c r="F170" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>7</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C171" s="3">
+        <v>1</v>
+      </c>
+      <c r="D171" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E167" s="1" t="s">
+      <c r="E171" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F167" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6">
-      <c r="A168">
-        <v>7</v>
-      </c>
-      <c r="B168" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C168" s="3">
-        <v>1</v>
-      </c>
-      <c r="D168" s="1" t="s">
+      <c r="F171" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>7</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C172" s="3">
+        <v>1</v>
+      </c>
+      <c r="D172" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E168" s="1" t="s">
+      <c r="E172" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F168" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6">
-      <c r="A169">
-        <v>7</v>
-      </c>
-      <c r="B169" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C169" s="3">
-        <v>1</v>
-      </c>
-      <c r="D169" s="1" t="s">
+      <c r="F172" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A173">
+        <v>7</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C173" s="3">
+        <v>1</v>
+      </c>
+      <c r="D173" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E169" s="1" t="s">
+      <c r="E173" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F169" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" ht="15">
-      <c r="A170">
-        <v>7</v>
-      </c>
-      <c r="B170" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C170" s="3">
-        <v>1</v>
-      </c>
-      <c r="D170" s="1" t="s">
+      <c r="F173" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A174">
+        <v>7</v>
+      </c>
+      <c r="B174" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C174" s="3">
+        <v>1</v>
+      </c>
+      <c r="D174" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E170" s="1" t="s">
+      <c r="E174" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F170" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6">
-      <c r="A171">
-        <v>7</v>
-      </c>
-      <c r="B171" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C171" s="3">
-        <v>1</v>
-      </c>
-      <c r="D171" s="1" t="s">
+      <c r="F174" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A175">
+        <v>7</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C175" s="3">
+        <v>1</v>
+      </c>
+      <c r="D175" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E171" s="1" t="s">
+      <c r="E175" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F171" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6">
-      <c r="A172">
-        <v>7</v>
-      </c>
-      <c r="B172" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C172" s="3">
-        <v>1</v>
-      </c>
-      <c r="D172" s="1" t="s">
+      <c r="F175" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A176">
+        <v>7</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C176" s="3">
+        <v>1</v>
+      </c>
+      <c r="D176" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E172" s="1" t="s">
+      <c r="E176" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F172" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6">
-      <c r="A173">
-        <v>7</v>
-      </c>
-      <c r="B173" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C173" s="3">
-        <v>1</v>
-      </c>
-      <c r="D173" s="1" t="s">
+      <c r="F176" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A177">
+        <v>7</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C177" s="3">
+        <v>1</v>
+      </c>
+      <c r="D177" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E173" s="1" t="s">
+      <c r="E177" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F173" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6">
-      <c r="A174">
-        <v>7</v>
-      </c>
-      <c r="B174" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C174" s="3">
-        <v>1</v>
-      </c>
-      <c r="D174" s="1" t="s">
+      <c r="F177" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A178">
+        <v>7</v>
+      </c>
+      <c r="B178" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C178" s="3">
+        <v>1</v>
+      </c>
+      <c r="D178" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E174" s="1" t="s">
+      <c r="E178" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F174" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6">
-      <c r="A175">
-        <v>7</v>
-      </c>
-      <c r="B175" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C175" s="3">
-        <v>1</v>
-      </c>
-      <c r="D175" s="1" t="s">
+      <c r="F178" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A179">
+        <v>7</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C179" s="3">
+        <v>1</v>
+      </c>
+      <c r="D179" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E175" s="1" t="s">
+      <c r="E179" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F175" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6">
-      <c r="A176">
-        <v>7</v>
-      </c>
-      <c r="B176" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C176" s="3">
-        <v>1</v>
-      </c>
-      <c r="D176" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E176" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F176" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6">
-      <c r="A177">
-        <v>0</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C177" s="3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6">
-      <c r="A178">
-        <v>8</v>
-      </c>
-      <c r="B178" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C178" s="3">
-        <v>1</v>
-      </c>
-      <c r="D178" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F178" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6">
-      <c r="A179">
-        <v>8</v>
-      </c>
-      <c r="B179" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C179" s="3">
-        <v>1</v>
-      </c>
-      <c r="D179" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E179" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="F179" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:6">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="C180" s="3">
         <v>1</v>
@@ -4013,33 +4037,24 @@
         <v>38</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F180" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:6">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181">
-        <v>8</v>
-      </c>
-      <c r="B181" s="4" t="s">
-        <v>55</v>
+        <v>0</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C181" s="3">
-        <v>1</v>
-      </c>
-      <c r="D181" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F181" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>8</v>
       </c>
@@ -4050,16 +4065,16 @@
         <v>1</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F182" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:6">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>8</v>
       </c>
@@ -4070,16 +4085,16 @@
         <v>1</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F183" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:6">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>8</v>
       </c>
@@ -4090,16 +4105,16 @@
         <v>1</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F184" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:6">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>8</v>
       </c>
@@ -4110,16 +4125,16 @@
         <v>1</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="F185" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:6">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>8</v>
       </c>
@@ -4130,16 +4145,16 @@
         <v>1</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F186" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:6">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>8</v>
       </c>
@@ -4150,16 +4165,16 @@
         <v>1</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="F187" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:6">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>8</v>
       </c>
@@ -4170,16 +4185,16 @@
         <v>1</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F188" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:6">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>8</v>
       </c>
@@ -4190,16 +4205,16 @@
         <v>1</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F189" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:6">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>8</v>
       </c>
@@ -4210,16 +4225,16 @@
         <v>1</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="F190" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:6">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>8</v>
       </c>
@@ -4230,16 +4245,16 @@
         <v>1</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F191" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:6">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>8</v>
       </c>
@@ -4250,16 +4265,16 @@
         <v>1</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F192" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:6">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>8</v>
       </c>
@@ -4270,16 +4285,16 @@
         <v>1</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F193" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:6">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>8</v>
       </c>
@@ -4290,16 +4305,16 @@
         <v>1</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="F194" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:6">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>8</v>
       </c>
@@ -4310,16 +4325,16 @@
         <v>1</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F195" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:6">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>8</v>
       </c>
@@ -4330,16 +4345,16 @@
         <v>1</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F196" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:6">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>8</v>
       </c>
@@ -4350,16 +4365,16 @@
         <v>1</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F197" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:6">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>8</v>
       </c>
@@ -4370,16 +4385,16 @@
         <v>1</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F198" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:6">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>8</v>
       </c>
@@ -4390,16 +4405,16 @@
         <v>1</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="F199" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:6">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>8</v>
       </c>
@@ -4410,16 +4425,16 @@
         <v>1</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F200" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:6">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>8</v>
       </c>
@@ -4430,23 +4445,103 @@
         <v>1</v>
       </c>
       <c r="D201" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F201" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A202">
+        <v>8</v>
+      </c>
+      <c r="B202" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C202" s="3">
+        <v>1</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F202" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A203">
+        <v>8</v>
+      </c>
+      <c r="B203" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C203" s="3">
+        <v>1</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F203" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A204">
+        <v>8</v>
+      </c>
+      <c r="B204" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C204" s="3">
+        <v>1</v>
+      </c>
+      <c r="D204" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E201" s="1" t="s">
+      <c r="E204" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F201" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6">
-      <c r="A202">
-        <v>0</v>
-      </c>
-      <c r="B202" s="1" t="s">
+      <c r="F204" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A205">
+        <v>8</v>
+      </c>
+      <c r="B205" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C205" s="3">
+        <v>1</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F205" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A206">
+        <v>0</v>
+      </c>
+      <c r="B206" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C202" s="3">
+      <c r="C206" s="3">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated order files with png
</commit_message>
<xml_diff>
--- a/Experiment/Orders_PILOT/PAR01_RUN02.xlsx
+++ b/Experiment/Orders_PILOT/PAR01_RUN02.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdonnel9\Documents\GitHub\fMRI_3DFaces_MD_2021\Experiment\Orders_PILOT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kstubbs5\Documents\GitHub\fMRI_3DFaces_MD_2021\Experiment\Orders_PILOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -59,144 +59,6 @@
     <t>3D</t>
   </si>
   <si>
-    <t>Face8_L.jpg</t>
-  </si>
-  <si>
-    <t>Face8_R.jpg</t>
-  </si>
-  <si>
-    <t>Face17_L.jpg</t>
-  </si>
-  <si>
-    <t>Face17_R.jpg</t>
-  </si>
-  <si>
-    <t>Face6_L.jpg</t>
-  </si>
-  <si>
-    <t>Face6_R.jpg</t>
-  </si>
-  <si>
-    <t>Face23_L.jpg</t>
-  </si>
-  <si>
-    <t>Face23_R.jpg</t>
-  </si>
-  <si>
-    <t>Face20_L.jpg</t>
-  </si>
-  <si>
-    <t>Face20_R.jpg</t>
-  </si>
-  <si>
-    <t>Face12_L.jpg</t>
-  </si>
-  <si>
-    <t>Face12_R.jpg</t>
-  </si>
-  <si>
-    <t>Face1_L.jpg</t>
-  </si>
-  <si>
-    <t>Face1_R.jpg</t>
-  </si>
-  <si>
-    <t>Face5_L.jpg</t>
-  </si>
-  <si>
-    <t>Face5_R.jpg</t>
-  </si>
-  <si>
-    <t>Face22_L.jpg</t>
-  </si>
-  <si>
-    <t>Face22_R.jpg</t>
-  </si>
-  <si>
-    <t>Face16_L.jpg</t>
-  </si>
-  <si>
-    <t>Face16_R.jpg</t>
-  </si>
-  <si>
-    <t>Face7_L.jpg</t>
-  </si>
-  <si>
-    <t>Face7_R.jpg</t>
-  </si>
-  <si>
-    <t>Face15_L.jpg</t>
-  </si>
-  <si>
-    <t>Face15_R.jpg</t>
-  </si>
-  <si>
-    <t>Face14_L.jpg</t>
-  </si>
-  <si>
-    <t>Face14_R.jpg</t>
-  </si>
-  <si>
-    <t>Face4_L.jpg</t>
-  </si>
-  <si>
-    <t>Face4_R.jpg</t>
-  </si>
-  <si>
-    <t>Face19_L.jpg</t>
-  </si>
-  <si>
-    <t>Face19_R.jpg</t>
-  </si>
-  <si>
-    <t>Face9_L.jpg</t>
-  </si>
-  <si>
-    <t>Face9_R.jpg</t>
-  </si>
-  <si>
-    <t>Face11_L.jpg</t>
-  </si>
-  <si>
-    <t>Face11_R.jpg</t>
-  </si>
-  <si>
-    <t>Face18_L.jpg</t>
-  </si>
-  <si>
-    <t>Face18_R.jpg</t>
-  </si>
-  <si>
-    <t>Face13_L.jpg</t>
-  </si>
-  <si>
-    <t>Face13_R.jpg</t>
-  </si>
-  <si>
-    <t>Face10_L.jpg</t>
-  </si>
-  <si>
-    <t>Face10_R.jpg</t>
-  </si>
-  <si>
-    <t>Face2_L.jpg</t>
-  </si>
-  <si>
-    <t>Face2_R.jpg</t>
-  </si>
-  <si>
-    <t>Face21_L.jpg</t>
-  </si>
-  <si>
-    <t>Face21_R.jpg</t>
-  </si>
-  <si>
-    <t>Face3_L.jpg</t>
-  </si>
-  <si>
-    <t>Face3_R.jpg</t>
-  </si>
-  <si>
     <t>MonocL</t>
   </si>
   <si>
@@ -209,10 +71,148 @@
     <t>CUE</t>
   </si>
   <si>
-    <t>CoverCue.jpg</t>
-  </si>
-  <si>
-    <t>UncoverCue.jpg</t>
+    <t>Face15_L.png</t>
+  </si>
+  <si>
+    <t>Face15_R.png</t>
+  </si>
+  <si>
+    <t>Face7_L.png</t>
+  </si>
+  <si>
+    <t>Face7_R.png</t>
+  </si>
+  <si>
+    <t>Face8_L.png</t>
+  </si>
+  <si>
+    <t>Face8_R.png</t>
+  </si>
+  <si>
+    <t>Face2_L.png</t>
+  </si>
+  <si>
+    <t>Face2_R.png</t>
+  </si>
+  <si>
+    <t>Face17_L.png</t>
+  </si>
+  <si>
+    <t>Face17_R.png</t>
+  </si>
+  <si>
+    <t>Face16_L.png</t>
+  </si>
+  <si>
+    <t>Face16_R.png</t>
+  </si>
+  <si>
+    <t>Face20_L.png</t>
+  </si>
+  <si>
+    <t>Face20_R.png</t>
+  </si>
+  <si>
+    <t>Face5_L.png</t>
+  </si>
+  <si>
+    <t>Face5_R.png</t>
+  </si>
+  <si>
+    <t>Face22_L.png</t>
+  </si>
+  <si>
+    <t>Face22_R.png</t>
+  </si>
+  <si>
+    <t>Face1_L.png</t>
+  </si>
+  <si>
+    <t>Face1_R.png</t>
+  </si>
+  <si>
+    <t>Face13_L.png</t>
+  </si>
+  <si>
+    <t>Face13_R.png</t>
+  </si>
+  <si>
+    <t>Face14_L.png</t>
+  </si>
+  <si>
+    <t>Face14_R.png</t>
+  </si>
+  <si>
+    <t>Face3_L.png</t>
+  </si>
+  <si>
+    <t>Face3_R.png</t>
+  </si>
+  <si>
+    <t>Face4_L.png</t>
+  </si>
+  <si>
+    <t>Face4_R.png</t>
+  </si>
+  <si>
+    <t>Face21_L.png</t>
+  </si>
+  <si>
+    <t>Face21_R.png</t>
+  </si>
+  <si>
+    <t>Face10_L.png</t>
+  </si>
+  <si>
+    <t>Face10_R.png</t>
+  </si>
+  <si>
+    <t>Face11_L.png</t>
+  </si>
+  <si>
+    <t>Face11_R.png</t>
+  </si>
+  <si>
+    <t>Face19_L.png</t>
+  </si>
+  <si>
+    <t>Face19_R.png</t>
+  </si>
+  <si>
+    <t>Face6_L.png</t>
+  </si>
+  <si>
+    <t>Face6_R.png</t>
+  </si>
+  <si>
+    <t>Face12_L.png</t>
+  </si>
+  <si>
+    <t>Face12_R.png</t>
+  </si>
+  <si>
+    <t>Face9_L.png</t>
+  </si>
+  <si>
+    <t>Face9_R.png</t>
+  </si>
+  <si>
+    <t>Face18_L.png</t>
+  </si>
+  <si>
+    <t>Face18_R.png</t>
+  </si>
+  <si>
+    <t>Face23_L.png</t>
+  </si>
+  <si>
+    <t>Face23_R.png</t>
+  </si>
+  <si>
+    <t>CoverCue.png</t>
+  </si>
+  <si>
+    <t>UncoverCue.png</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
   <dimension ref="A1:F206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K180" sqref="K180"/>
+      <selection sqref="A1:F206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,10 +637,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -657,10 +657,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -677,10 +677,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -697,10 +697,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -717,10 +717,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -737,10 +737,10 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -757,10 +757,10 @@
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -777,10 +777,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F10" t="b">
         <v>0</v>
@@ -797,10 +797,10 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F11" t="b">
         <v>0</v>
@@ -817,10 +817,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F12" t="b">
         <v>0</v>
@@ -837,10 +837,10 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -857,10 +857,10 @@
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F14" t="b">
         <v>1</v>
@@ -877,10 +877,10 @@
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -897,10 +897,10 @@
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="F16" t="b">
         <v>0</v>
@@ -917,10 +917,10 @@
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F17" t="b">
         <v>0</v>
@@ -937,10 +937,10 @@
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F18" t="b">
         <v>0</v>
@@ -957,10 +957,10 @@
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -977,10 +977,10 @@
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F20" t="b">
         <v>0</v>
@@ -997,10 +997,10 @@
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
@@ -1017,10 +1017,10 @@
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
@@ -1037,10 +1037,10 @@
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -1057,10 +1057,10 @@
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
@@ -1077,10 +1077,10 @@
         <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -1097,10 +1097,10 @@
         <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
@@ -1111,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="C27" s="3">
         <v>5</v>
@@ -1144,16 +1144,16 @@
         <v>2</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C29" s="3">
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
@@ -1164,16 +1164,16 @@
         <v>2</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C30" s="3">
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
@@ -1184,16 +1184,16 @@
         <v>2</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C31" s="3">
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
@@ -1204,16 +1204,16 @@
         <v>2</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C32" s="3">
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
@@ -1224,16 +1224,16 @@
         <v>2</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C33" s="3">
         <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
@@ -1244,16 +1244,16 @@
         <v>2</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C34" s="3">
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
@@ -1264,16 +1264,16 @@
         <v>2</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C35" s="3">
         <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
@@ -1284,16 +1284,16 @@
         <v>2</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C36" s="3">
         <v>1</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
@@ -1304,16 +1304,16 @@
         <v>2</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C37" s="3">
         <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
@@ -1324,16 +1324,16 @@
         <v>2</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C38" s="3">
         <v>1</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
@@ -1344,16 +1344,16 @@
         <v>2</v>
       </c>
       <c r="B39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="3">
-        <v>1</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="E39" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
@@ -1364,16 +1364,16 @@
         <v>2</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C40" s="3">
         <v>1</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
@@ -1384,16 +1384,16 @@
         <v>2</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C41" s="3">
         <v>1</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
@@ -1404,16 +1404,16 @@
         <v>2</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C42" s="3">
         <v>1</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
@@ -1424,16 +1424,16 @@
         <v>2</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C43" s="3">
         <v>1</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F43" t="b">
         <v>0</v>
@@ -1444,16 +1444,16 @@
         <v>2</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C44" s="3">
         <v>1</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F44" t="b">
         <v>0</v>
@@ -1464,16 +1464,16 @@
         <v>2</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C45" s="3">
         <v>1</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F45" t="b">
         <v>0</v>
@@ -1484,16 +1484,16 @@
         <v>2</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C46" s="3">
         <v>1</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F46" t="b">
         <v>1</v>
@@ -1504,16 +1504,16 @@
         <v>2</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C47" s="3">
         <v>1</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F47" t="b">
         <v>0</v>
@@ -1524,16 +1524,16 @@
         <v>2</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C48" s="3">
         <v>1</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F48" t="b">
         <v>0</v>
@@ -1544,16 +1544,16 @@
         <v>2</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C49" s="3">
         <v>1</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F49" t="b">
         <v>0</v>
@@ -1564,16 +1564,16 @@
         <v>2</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C50" s="3">
         <v>1</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="F50" t="b">
         <v>0</v>
@@ -1584,16 +1584,16 @@
         <v>2</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C51" s="3">
         <v>1</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F51" t="b">
         <v>0</v>
@@ -1604,16 +1604,16 @@
         <v>2</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C52" s="3">
         <v>1</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F52" t="b">
         <v>0</v>
@@ -1624,7 +1624,7 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="C53" s="3">
         <v>5</v>
@@ -1655,16 +1655,16 @@
         <v>3</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C55" s="3">
         <v>1</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F55" t="b">
         <v>0</v>
@@ -1675,16 +1675,16 @@
         <v>3</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C56" s="3">
         <v>1</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F56" t="b">
         <v>0</v>
@@ -1695,16 +1695,16 @@
         <v>3</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C57" s="3">
         <v>1</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F57" t="b">
         <v>1</v>
@@ -1715,16 +1715,16 @@
         <v>3</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C58" s="3">
         <v>1</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F58" t="b">
         <v>0</v>
@@ -1735,16 +1735,16 @@
         <v>3</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C59" s="3">
         <v>1</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F59" t="b">
         <v>0</v>
@@ -1755,16 +1755,16 @@
         <v>3</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C60" s="3">
         <v>1</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="F60" t="b">
         <v>0</v>
@@ -1775,16 +1775,16 @@
         <v>3</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C61" s="3">
         <v>1</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F61" t="b">
         <v>0</v>
@@ -1795,16 +1795,16 @@
         <v>3</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C62" s="3">
         <v>1</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F62" t="b">
         <v>0</v>
@@ -1815,16 +1815,16 @@
         <v>3</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C63" s="3">
         <v>1</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F63" t="b">
         <v>0</v>
@@ -1835,16 +1835,16 @@
         <v>3</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C64" s="3">
         <v>1</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F64" t="b">
         <v>0</v>
@@ -1855,16 +1855,16 @@
         <v>3</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C65" s="3">
         <v>1</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="F65" t="b">
         <v>0</v>
@@ -1875,16 +1875,16 @@
         <v>3</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C66" s="3">
         <v>1</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F66" t="b">
         <v>0</v>
@@ -1895,16 +1895,16 @@
         <v>3</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C67" s="3">
         <v>1</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F67" t="b">
         <v>0</v>
@@ -1915,16 +1915,16 @@
         <v>3</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C68" s="3">
         <v>1</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="F68" t="b">
         <v>0</v>
@@ -1935,16 +1935,16 @@
         <v>3</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C69" s="3">
         <v>1</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="F69" t="b">
         <v>0</v>
@@ -1955,16 +1955,16 @@
         <v>3</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C70" s="3">
         <v>1</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F70" t="b">
         <v>0</v>
@@ -1975,16 +1975,16 @@
         <v>3</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C71" s="3">
         <v>1</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F71" t="b">
         <v>0</v>
@@ -1995,16 +1995,16 @@
         <v>3</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C72" s="3">
         <v>1</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="F72" t="b">
         <v>0</v>
@@ -2015,16 +2015,16 @@
         <v>3</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C73" s="3">
         <v>1</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F73" t="b">
         <v>0</v>
@@ -2035,16 +2035,16 @@
         <v>3</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C74" s="3">
         <v>1</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F74" t="b">
         <v>0</v>
@@ -2055,16 +2055,16 @@
         <v>3</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C75" s="3">
         <v>1</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="F75" t="b">
         <v>0</v>
@@ -2075,16 +2075,16 @@
         <v>3</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C76" s="3">
         <v>1</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F76" t="b">
         <v>0</v>
@@ -2095,16 +2095,16 @@
         <v>3</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C77" s="3">
         <v>1</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F77" t="b">
         <v>0</v>
@@ -2115,16 +2115,16 @@
         <v>3</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C78" s="3">
         <v>1</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F78" t="b">
         <v>0</v>
@@ -2146,16 +2146,16 @@
         <v>4</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C80" s="3">
         <v>1</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F80" t="b">
         <v>0</v>
@@ -2166,16 +2166,16 @@
         <v>4</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C81" s="3">
         <v>1</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="F81" t="b">
         <v>0</v>
@@ -2186,16 +2186,16 @@
         <v>4</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C82" s="3">
         <v>1</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F82" t="b">
         <v>0</v>
@@ -2206,16 +2206,16 @@
         <v>4</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C83" s="3">
         <v>1</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F83" t="b">
         <v>0</v>
@@ -2226,16 +2226,16 @@
         <v>4</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C84" s="3">
         <v>1</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F84" t="b">
         <v>0</v>
@@ -2246,16 +2246,16 @@
         <v>4</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C85" s="3">
         <v>1</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F85" t="b">
         <v>0</v>
@@ -2266,16 +2266,16 @@
         <v>4</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C86" s="3">
         <v>1</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F86" t="b">
         <v>0</v>
@@ -2286,16 +2286,16 @@
         <v>4</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C87" s="3">
         <v>1</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F87" t="b">
         <v>0</v>
@@ -2306,16 +2306,16 @@
         <v>4</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C88" s="3">
         <v>1</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="F88" t="b">
         <v>0</v>
@@ -2326,16 +2326,16 @@
         <v>4</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C89" s="3">
         <v>1</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="F89" t="b">
         <v>0</v>
@@ -2346,16 +2346,16 @@
         <v>4</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C90" s="3">
         <v>1</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F90" t="b">
         <v>0</v>
@@ -2366,16 +2366,16 @@
         <v>4</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C91" s="3">
         <v>1</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F91" t="b">
         <v>0</v>
@@ -2386,16 +2386,16 @@
         <v>4</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C92" s="3">
         <v>1</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F92" t="b">
         <v>0</v>
@@ -2406,16 +2406,16 @@
         <v>4</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C93" s="3">
         <v>1</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F93" t="b">
         <v>0</v>
@@ -2426,16 +2426,16 @@
         <v>4</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C94" s="3">
         <v>1</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="F94" t="b">
         <v>0</v>
@@ -2446,16 +2446,16 @@
         <v>4</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C95" s="3">
         <v>1</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F95" t="b">
         <v>0</v>
@@ -2466,16 +2466,16 @@
         <v>4</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C96" s="3">
         <v>1</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F96" t="b">
         <v>1</v>
@@ -2486,16 +2486,16 @@
         <v>4</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C97" s="3">
         <v>1</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F97" t="b">
         <v>0</v>
@@ -2506,16 +2506,16 @@
         <v>4</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C98" s="3">
         <v>1</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="F98" t="b">
         <v>0</v>
@@ -2526,16 +2526,16 @@
         <v>4</v>
       </c>
       <c r="B99" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C99" s="3">
+        <v>1</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E99" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C99" s="3">
-        <v>1</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="F99" t="b">
         <v>0</v>
@@ -2546,16 +2546,16 @@
         <v>4</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C100" s="3">
         <v>1</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F100" t="b">
         <v>0</v>
@@ -2566,16 +2566,16 @@
         <v>4</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C101" s="3">
         <v>1</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F101" t="b">
         <v>0</v>
@@ -2586,16 +2586,16 @@
         <v>4</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C102" s="3">
         <v>1</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F102" t="b">
         <v>0</v>
@@ -2606,16 +2606,16 @@
         <v>4</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C103" s="3">
         <v>1</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F103" t="b">
         <v>0</v>
@@ -2626,7 +2626,7 @@
         <v>0</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="C104" s="3">
         <v>5</v>
@@ -2659,16 +2659,16 @@
         <v>5</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C106" s="3">
         <v>1</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F106" t="b">
         <v>0</v>
@@ -2679,16 +2679,16 @@
         <v>5</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C107" s="3">
         <v>1</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F107" t="b">
         <v>0</v>
@@ -2699,16 +2699,16 @@
         <v>5</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C108" s="3">
         <v>1</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F108" t="b">
         <v>0</v>
@@ -2719,16 +2719,16 @@
         <v>5</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C109" s="3">
         <v>1</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F109" t="b">
         <v>0</v>
@@ -2739,16 +2739,16 @@
         <v>5</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C110" s="3">
         <v>1</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="F110" t="b">
         <v>0</v>
@@ -2759,16 +2759,16 @@
         <v>5</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C111" s="3">
         <v>1</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F111" t="b">
         <v>0</v>
@@ -2779,16 +2779,16 @@
         <v>5</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C112" s="3">
         <v>1</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F112" t="b">
         <v>0</v>
@@ -2799,16 +2799,16 @@
         <v>5</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C113" s="3">
         <v>1</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="F113" t="b">
         <v>0</v>
@@ -2819,16 +2819,16 @@
         <v>5</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C114" s="3">
         <v>1</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F114" t="b">
         <v>0</v>
@@ -2839,16 +2839,16 @@
         <v>5</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C115" s="3">
         <v>1</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F115" t="b">
         <v>0</v>
@@ -2859,16 +2859,16 @@
         <v>5</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C116" s="3">
         <v>1</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F116" t="b">
         <v>0</v>
@@ -2879,16 +2879,16 @@
         <v>5</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C117" s="3">
         <v>1</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F117" t="b">
         <v>0</v>
@@ -2899,16 +2899,16 @@
         <v>5</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C118" s="3">
         <v>1</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F118" t="b">
         <v>0</v>
@@ -2919,16 +2919,16 @@
         <v>5</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C119" s="3">
         <v>1</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F119" t="b">
         <v>1</v>
@@ -2939,16 +2939,16 @@
         <v>5</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C120" s="3">
         <v>1</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F120" t="b">
         <v>0</v>
@@ -2959,16 +2959,16 @@
         <v>5</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C121" s="3">
         <v>1</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F121" t="b">
         <v>0</v>
@@ -2979,16 +2979,16 @@
         <v>5</v>
       </c>
       <c r="B122" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C122" s="3">
+        <v>1</v>
+      </c>
+      <c r="D122" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C122" s="3">
-        <v>1</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="E122" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F122" t="b">
         <v>0</v>
@@ -2999,16 +2999,16 @@
         <v>5</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C123" s="3">
         <v>1</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="F123" t="b">
         <v>0</v>
@@ -3019,16 +3019,16 @@
         <v>5</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C124" s="3">
         <v>1</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F124" t="b">
         <v>0</v>
@@ -3039,16 +3039,16 @@
         <v>5</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C125" s="3">
         <v>1</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="F125" t="b">
         <v>0</v>
@@ -3059,16 +3059,16 @@
         <v>5</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C126" s="3">
         <v>1</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F126" t="b">
         <v>0</v>
@@ -3079,16 +3079,16 @@
         <v>5</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C127" s="3">
         <v>1</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F127" t="b">
         <v>0</v>
@@ -3099,16 +3099,16 @@
         <v>5</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C128" s="3">
         <v>1</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="F128" t="b">
         <v>0</v>
@@ -3119,16 +3119,16 @@
         <v>5</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C129" s="3">
         <v>1</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="F129" t="b">
         <v>0</v>
@@ -3139,7 +3139,7 @@
         <v>0</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="C130" s="3">
         <v>5</v>
@@ -3172,16 +3172,16 @@
         <v>6</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C132" s="3">
         <v>1</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="F132" t="b">
         <v>0</v>
@@ -3192,16 +3192,16 @@
         <v>6</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C133" s="3">
         <v>1</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F133" t="b">
         <v>0</v>
@@ -3212,16 +3212,16 @@
         <v>6</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C134" s="3">
         <v>1</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F134" t="b">
         <v>0</v>
@@ -3232,16 +3232,16 @@
         <v>6</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C135" s="3">
         <v>1</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F135" t="b">
         <v>0</v>
@@ -3252,16 +3252,16 @@
         <v>6</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C136" s="3">
         <v>1</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F136" t="b">
         <v>0</v>
@@ -3272,16 +3272,16 @@
         <v>6</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C137" s="3">
         <v>1</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F137" t="b">
         <v>0</v>
@@ -3292,16 +3292,16 @@
         <v>6</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C138" s="3">
         <v>1</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F138" t="b">
         <v>0</v>
@@ -3312,16 +3312,16 @@
         <v>6</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C139" s="3">
         <v>1</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F139" t="b">
         <v>0</v>
@@ -3332,16 +3332,16 @@
         <v>6</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C140" s="3">
         <v>1</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F140" t="b">
         <v>0</v>
@@ -3352,16 +3352,16 @@
         <v>6</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C141" s="3">
         <v>1</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F141" t="b">
         <v>0</v>
@@ -3372,16 +3372,16 @@
         <v>6</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C142" s="3">
         <v>1</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F142" t="b">
         <v>0</v>
@@ -3392,16 +3392,16 @@
         <v>6</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C143" s="3">
         <v>1</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="F143" t="b">
         <v>0</v>
@@ -3412,16 +3412,16 @@
         <v>6</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C144" s="3">
         <v>1</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="F144" t="b">
         <v>1</v>
@@ -3432,16 +3432,16 @@
         <v>6</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C145" s="3">
         <v>1</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F145" t="b">
         <v>0</v>
@@ -3452,16 +3452,16 @@
         <v>6</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C146" s="3">
         <v>1</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="F146" t="b">
         <v>0</v>
@@ -3472,16 +3472,16 @@
         <v>6</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C147" s="3">
         <v>1</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F147" t="b">
         <v>0</v>
@@ -3492,16 +3492,16 @@
         <v>6</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C148" s="3">
         <v>1</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F148" t="b">
         <v>0</v>
@@ -3512,16 +3512,16 @@
         <v>6</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C149" s="3">
         <v>1</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F149" t="b">
         <v>0</v>
@@ -3532,16 +3532,16 @@
         <v>6</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C150" s="3">
         <v>1</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F150" t="b">
         <v>0</v>
@@ -3552,16 +3552,16 @@
         <v>6</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C151" s="3">
         <v>1</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F151" t="b">
         <v>0</v>
@@ -3572,16 +3572,16 @@
         <v>6</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C152" s="3">
         <v>1</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F152" t="b">
         <v>0</v>
@@ -3592,16 +3592,16 @@
         <v>6</v>
       </c>
       <c r="B153" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C153" s="3">
+        <v>1</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E153" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C153" s="3">
-        <v>1</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E153" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="F153" t="b">
         <v>0</v>
@@ -3612,16 +3612,16 @@
         <v>6</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C154" s="3">
         <v>1</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="F154" t="b">
         <v>0</v>
@@ -3632,16 +3632,16 @@
         <v>6</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C155" s="3">
         <v>1</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="F155" t="b">
         <v>0</v>
@@ -3669,10 +3669,10 @@
         <v>1</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="F157" t="b">
         <v>0</v>
@@ -3689,10 +3689,10 @@
         <v>1</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="F158" t="b">
         <v>0</v>
@@ -3709,10 +3709,10 @@
         <v>1</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F159" t="b">
         <v>0</v>
@@ -3729,10 +3729,10 @@
         <v>1</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F160" t="b">
         <v>0</v>
@@ -3749,10 +3749,10 @@
         <v>1</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F161" t="b">
         <v>0</v>
@@ -3769,10 +3769,10 @@
         <v>1</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F162" t="b">
         <v>1</v>
@@ -3789,10 +3789,10 @@
         <v>1</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F163" t="b">
         <v>0</v>
@@ -3809,10 +3809,10 @@
         <v>1</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F164" t="b">
         <v>0</v>
@@ -3829,10 +3829,10 @@
         <v>1</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F165" t="b">
         <v>0</v>
@@ -3849,10 +3849,10 @@
         <v>1</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="F166" t="b">
         <v>0</v>
@@ -3869,10 +3869,10 @@
         <v>1</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="F167" t="b">
         <v>0</v>
@@ -3889,10 +3889,10 @@
         <v>1</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F168" t="b">
         <v>0</v>
@@ -3909,10 +3909,10 @@
         <v>1</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F169" t="b">
         <v>0</v>
@@ -3929,10 +3929,10 @@
         <v>1</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F170" t="b">
         <v>0</v>
@@ -3949,10 +3949,10 @@
         <v>1</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F171" t="b">
         <v>0</v>
@@ -3969,10 +3969,10 @@
         <v>1</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="F172" t="b">
         <v>0</v>
@@ -3989,10 +3989,10 @@
         <v>1</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="F173" t="b">
         <v>0</v>
@@ -4009,10 +4009,10 @@
         <v>1</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F174" t="b">
         <v>0</v>
@@ -4029,10 +4029,10 @@
         <v>1</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="F175" t="b">
         <v>0</v>
@@ -4049,10 +4049,10 @@
         <v>1</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F176" t="b">
         <v>0</v>
@@ -4069,10 +4069,10 @@
         <v>1</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F177" t="b">
         <v>0</v>
@@ -4089,10 +4089,10 @@
         <v>1</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="F178" t="b">
         <v>0</v>
@@ -4109,10 +4109,10 @@
         <v>1</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F179" t="b">
         <v>0</v>
@@ -4129,10 +4129,10 @@
         <v>1</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="F180" t="b">
         <v>0</v>
@@ -4154,16 +4154,16 @@
         <v>8</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C182" s="3">
         <v>1</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F182" t="b">
         <v>0</v>
@@ -4174,16 +4174,16 @@
         <v>8</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C183" s="3">
         <v>1</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F183" t="b">
         <v>0</v>
@@ -4194,16 +4194,16 @@
         <v>8</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C184" s="3">
         <v>1</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="F184" t="b">
         <v>0</v>
@@ -4214,16 +4214,16 @@
         <v>8</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C185" s="3">
         <v>1</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F185" t="b">
         <v>0</v>
@@ -4234,16 +4234,16 @@
         <v>8</v>
       </c>
       <c r="B186" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C186" s="3">
         <v>1</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F186" t="b">
         <v>0</v>
@@ -4254,16 +4254,16 @@
         <v>8</v>
       </c>
       <c r="B187" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C187" s="3">
         <v>1</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F187" t="b">
         <v>0</v>
@@ -4274,16 +4274,16 @@
         <v>8</v>
       </c>
       <c r="B188" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C188" s="3">
         <v>1</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F188" t="b">
         <v>0</v>
@@ -4294,16 +4294,16 @@
         <v>8</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C189" s="3">
         <v>1</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F189" t="b">
         <v>0</v>
@@ -4314,16 +4314,16 @@
         <v>8</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C190" s="3">
         <v>1</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F190" t="b">
         <v>0</v>
@@ -4334,16 +4334,16 @@
         <v>8</v>
       </c>
       <c r="B191" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C191" s="3">
         <v>1</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="F191" t="b">
         <v>0</v>
@@ -4354,16 +4354,16 @@
         <v>8</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C192" s="3">
         <v>1</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F192" t="b">
         <v>0</v>
@@ -4374,16 +4374,16 @@
         <v>8</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C193" s="3">
         <v>1</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F193" t="b">
         <v>1</v>
@@ -4394,16 +4394,16 @@
         <v>8</v>
       </c>
       <c r="B194" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C194" s="3">
         <v>1</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="F194" t="b">
         <v>0</v>
@@ -4414,16 +4414,16 @@
         <v>8</v>
       </c>
       <c r="B195" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C195" s="3">
         <v>1</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F195" t="b">
         <v>0</v>
@@ -4434,16 +4434,16 @@
         <v>8</v>
       </c>
       <c r="B196" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C196" s="3">
         <v>1</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F196" t="b">
         <v>0</v>
@@ -4454,16 +4454,16 @@
         <v>8</v>
       </c>
       <c r="B197" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C197" s="3">
         <v>1</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F197" t="b">
         <v>0</v>
@@ -4474,16 +4474,16 @@
         <v>8</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C198" s="3">
         <v>1</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="F198" t="b">
         <v>0</v>
@@ -4494,16 +4494,16 @@
         <v>8</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C199" s="3">
         <v>1</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="F199" t="b">
         <v>0</v>
@@ -4514,16 +4514,16 @@
         <v>8</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C200" s="3">
         <v>1</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F200" t="b">
         <v>0</v>
@@ -4534,16 +4534,16 @@
         <v>8</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C201" s="3">
         <v>1</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F201" t="b">
         <v>0</v>
@@ -4554,16 +4554,16 @@
         <v>8</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C202" s="3">
         <v>1</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F202" t="b">
         <v>0</v>
@@ -4574,16 +4574,16 @@
         <v>8</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C203" s="3">
         <v>1</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F203" t="b">
         <v>0</v>
@@ -4594,16 +4594,16 @@
         <v>8</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C204" s="3">
         <v>1</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="F204" t="b">
         <v>0</v>
@@ -4614,16 +4614,16 @@
         <v>8</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C205" s="3">
         <v>1</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F205" t="b">
         <v>0</v>

</xml_diff>